<commit_message>
Created a file to sort all of the papers into respective folders. Changed GPT response from list to delimited string
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -14,57 +14,56 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
-  <si>
-    <t>3_MeV_Proton_Irradiation_of_Commercial_State_of_the_Art_Photonic_Mixer_Devices.pdf</t>
-  </si>
-  <si>
-    <t>RADON-5E_portable_pulsed_laser_simulator_description_qualification_technique_and_results_dosimetry_procedure.pdf</t>
-  </si>
-  <si>
-    <t>M. Grimm</t>
-  </si>
-  <si>
-    <t>EPC610</t>
-  </si>
-  <si>
-    <t>Photonic Mixer Device (PMD) sensor</t>
-  </si>
-  <si>
-    <t>Espros Photonics AG</t>
-  </si>
-  <si>
-    <t>SEE</t>
-  </si>
-  <si>
-    <t>Proton</t>
-  </si>
-  <si>
-    <t>3 MeV</t>
-  </si>
-  <si>
-    <t>1.5 · 10^11 p/cm^2</t>
-  </si>
-  <si>
-    <t>A.Y. Nikiforov</t>
-  </si>
-  <si>
-    <t>RADON-5E</t>
-  </si>
-  <si>
-    <t>portable pulsed laser simulator</t>
-  </si>
-  <si>
-    <t>Specialized Electronic Systems</t>
-  </si>
-  <si>
-    <t>Nd:YAG Laser</t>
-  </si>
-  <si>
-    <t>50-60 mJ</t>
-  </si>
-  <si>
-    <t>No</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+  <si>
+    <t>Papers_Sorted/SMD\Characterization_of_the_Effects_of_250_MeV_Proton-Induced_Total_Ionizing_Dose_and_Displacement_Damage_on_the_66266_Optocoupler.pdf</t>
+  </si>
+  <si>
+    <t>Papers_Sorted/SMD\Characterization_of_various_SEE_hardened_power_management_ICs.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S. Messenger </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 66266 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> optocoupler </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Micropac Industries, Inc. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type of radiation source: 250 MeV protons </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Failures: None </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> When: N/A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B. P. Alaskiewicz </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> IS-2100ARH </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> MOSFET driver IC </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Intersil Corporation </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SEE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Radiation Source Type: Au ions at 90.9MeV/mg/cm²
+Failures: No
+</t>
   </si>
 </sst>
 </file>
@@ -448,16 +447,10 @@
         <v>13</v>
       </c>
       <c r="F2" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s">
         <v>15</v>
-      </c>
-      <c r="I2" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added more comments for readability
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -14,12 +14,138 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
-  <si>
-    <t>Papers_Sorted/SMD\Characterization_of_the_Effects_of_250_MeV_Proton-Induced_Total_Ionizing_Dose_and_Displacement_Damage_on_the_66266_Optocoupler.pdf</t>
-  </si>
-  <si>
-    <t>Papers_Sorted/SMD\Characterization_of_various_SEE_hardened_power_management_ICs.pdf</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="56">
+  <si>
+    <t>Papers_Sorted/SMD/BJTs_in_Space_ELDRS_Experiment_on_NASA_Space_Environment_Testbed.pdf</t>
+  </si>
+  <si>
+    <t>Papers_Sorted/SMD/Characterization_of_various_SEE_hardened_power_management_ICs.pdf</t>
+  </si>
+  <si>
+    <t>Papers_Sorted/SMD/RADON-5E_portable_pulsed_laser_simulator_description_qualification_technique_and_results_dosimetry_procedure.pdf</t>
+  </si>
+  <si>
+    <t>Papers_Sorted/SMD/3_MeV_Proton_Irradiation_of_Commercial_State_of_the_Art_Photonic_Mixer_Devices.pdf</t>
+  </si>
+  <si>
+    <t>Papers_Sorted/SMD/A_16_MeV_nucleon_cocktail_for_heavy_ion_testing.pdf</t>
+  </si>
+  <si>
+    <t>Papers_Sorted/SMD/A_high_performance_Rad_hard_2-3_GHz_integer_N_CMOS_phase_lock_loop.pdf</t>
+  </si>
+  <si>
+    <t>Papers_Sorted/SMD/Characterization_of_the_Effects_of_250_MeV_Proton-Induced_Total_Ionizing_Dose_and_Displacement_Damage_on_the_66266_Optocoupler.pdf</t>
+  </si>
+  <si>
+    <t>Papers_Sorted/SMD/Radiation_Hardness_Performance_of_2_Gbit_LPDDR_SDRAM_Fabricated_on_Epitaxial_Wafer_for_Space_Applications.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G. Lyons </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> PE9601 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Phase Lock Loop (PLL) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Peregrine Semiconductor </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cobalt-60 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> N/A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A. R. Benedetto </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> N/A </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bipolar junction transistors (BJTs) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bipolar Junction Transistors (BJTs) </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Failures occurred from 8/02/2019 to 8/18/2019 and from 11/22/2020 to 1/06/2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B. P. Alaskiewicz </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> IS-2100ARH </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> MOSFET driver </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Intersil Corporation </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SEE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gold (Au), krypton (Kr), and argon (Ar) ions </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> No burnout or latchup observed, testing took place in August 2000.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A.Y. Nikiforov </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> RADON-5E Portable Pulsed Laser Simulator </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Portable Pulsed Laser Simulator </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Specialized Electronic Systems </t>
+  </si>
+  <si>
+    <t>Portable pulsed laser simulator, "RADON-SE" Ø Minor failures observed due to flash X-ray machine pulse-width differences. Specific times not mentioned.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M. Grimm </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> EPC610 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Photonic Mixer Device (PMD) sensor </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Espros Photonics AG </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 MeV Proton </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Communication failed at 1.5·10¹¹ p/cm², significant errors in internal temperature measurement at 7.0·10¹⁰ p/cm², current consumption increased by 80% up to 22 mA at 1.5·10¹¹ p/cm² </t>
+  </si>
+  <si>
+    <t xml:space="preserve">M. Y. Park </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SK Hynix 2 Gbit LPDDR SDRAM </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> LPDDR SDRAM </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SK Hynix </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heavy-ion (15 MeV/u, 38nm, SK Hynix 2Gb LPDDR) and Co-60 gamma-ray </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> No failures observed under test conditions up to maximum fluence and dose levels.</t>
   </si>
   <si>
     <t xml:space="preserve">S. Messenger </t>
@@ -34,36 +160,28 @@
     <t xml:space="preserve"> Micropac Industries, Inc. </t>
   </si>
   <si>
-    <t xml:space="preserve"> TID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Type of radiation source: 250 MeV protons </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Failures: None </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> When: N/A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B. P. Alaskiewicz </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> IS-2100ARH </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> MOSFET driver IC </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Intersil Corporation </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> SEE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Radiation Source Type: Au ions at 90.9MeV/mg/cm²
-Failures: No
-</t>
+    <t xml:space="preserve">250 MeV protons </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> no failures</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M.A. McMahan </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Part No. N/A </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> heavy ion cocktail </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Lawrence Berkeley National Laboratory </t>
+  </si>
+  <si>
+    <t xml:space="preserve">40Ar+14 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> None</t>
   </si>
 </sst>
 </file>
@@ -395,62 +513,215 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D1" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="E1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="F1" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="G1" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="H1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" t="s">
-        <v>14</v>
-      </c>
       <c r="G2" t="s">
-        <v>15</v>
+        <v>18</v>
+      </c>
+      <c r="H2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" t="s">
+        <v>42</v>
+      </c>
+      <c r="H6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" t="s">
+        <v>48</v>
+      </c>
+      <c r="H7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" t="s">
+        <v>53</v>
+      </c>
+      <c r="F8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" t="s">
+        <v>54</v>
+      </c>
+      <c r="H8" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>